<commit_message>
Lista matriz de trazabilidad
</commit_message>
<xml_diff>
--- a/Documentación/Tablas/8-3 Especificaciones de Diseño.xlsx
+++ b/Documentación/Tablas/8-3 Especificaciones de Diseño.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\Wet-DryPenguins\Documentación\Tablas\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856B19BD-D195-48AE-9462-ABAB3670D47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Especificaciones funcionales"/>
-    <sheet r:id="rId2" sheetId="2" name="Especificaciones de interfaz"/>
-    <sheet r:id="rId3" sheetId="3" name="Especificaciones dimensionales"/>
-    <sheet r:id="rId4" sheetId="4" name="Especificaciones de costo"/>
-    <sheet r:id="rId5" sheetId="5" name="Especificaciones de confiabilid"/>
-    <sheet r:id="rId6" sheetId="6" name="Especificaciones de operación"/>
+    <sheet name="Especificaciones funcionales" sheetId="1" r:id="rId1"/>
+    <sheet name="Especificaciones de interfaz" sheetId="2" r:id="rId2"/>
+    <sheet name="Especificaciones dimensionales" sheetId="3" r:id="rId3"/>
+    <sheet name="Especificaciones de costo" sheetId="4" r:id="rId4"/>
+    <sheet name="Especificaciones de confiabilid" sheetId="5" r:id="rId5"/>
+    <sheet name="Especificaciones de operación" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -40,9 +46,6 @@
     <t>El dispositivo debe poder operar en temperaturas entre 3°C y 50°C.</t>
   </si>
   <si>
-    <t>REQ-09</t>
-  </si>
-  <si>
     <t>P-F
 I-T</t>
   </si>
@@ -53,9 +56,6 @@
     <t>El dispositivo debe poder operar a una presión constante de hasta 8bar.</t>
   </si>
   <si>
-    <t>REQ-12</t>
-  </si>
-  <si>
     <t>IMP-OPE-3</t>
   </si>
   <si>
@@ -97,16 +97,10 @@
 I</t>
   </si>
   <si>
-    <t>INP-DIM-01</t>
-  </si>
-  <si>
     <t>El dispositivo debe poder asegurarse a la pata de un pingüino mediante precintos.</t>
   </si>
   <si>
     <t>REQ-01</t>
-  </si>
-  <si>
-    <t>INP-DIM-02</t>
   </si>
   <si>
     <t>El dispositivo debe tener dimensiones comprendidas dentro de un prisma de 40mm de ancho, 40mm
@@ -114,9 +108,6 @@
   </si>
   <si>
     <t>REQ-14</t>
-  </si>
-  <si>
-    <t>INP-DIM-03</t>
   </si>
   <si>
     <t>El dispositivo debe tener un peso menor a 10g, incluyendo circuito electrónico, fuente de energía y recubrimiento.</t>
@@ -297,14 +288,30 @@
     <t>A partir de los datos del dispositivo, debe poder
 obtenerse el patrón de comportamiento del
 pingüino bajo estudio.</t>
+  </si>
+  <si>
+    <t>REQ-09
+REQ-10</t>
+  </si>
+  <si>
+    <t>REQ-11
+REQ-12</t>
+  </si>
+  <si>
+    <t>IMP-DIM-01</t>
+  </si>
+  <si>
+    <t>IMP-DIM-02</t>
+  </si>
+  <si>
+    <t>IMP-DIM-03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +338,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -380,74 +393,68 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="17">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -458,10 +465,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -499,71 +506,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -591,7 +598,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -614,11 +621,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -627,13 +634,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -643,7 +650,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -652,7 +659,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -661,7 +668,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -669,10 +676,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -737,7 +744,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -747,21 +754,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="26.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="48.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="32.25">
-      <c r="A1" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="12"/>
+    <row r="1" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="13"/>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
@@ -775,209 +781,175 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="15" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="11" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="16" t="s">
+      <c r="D4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="E4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="5" t="s">
+      <c r="F4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="4" t="s">
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="32.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="17" t="s">
+      <c r="B5" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="5" t="s">
+      <c r="D5" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="F5" s="5" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="16" t="s">
+      <c r="G5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="17" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="5"/>
-      <c r="B6" s="17" t="s">
+      <c r="F7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="5" t="s">
+      <c r="G7" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="45.75">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="5" t="s">
+      <c r="F8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F9" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="48.75">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="18"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -990,7 +962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1000,13 +972,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="14" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1020,55 +992,50 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="48">
-      <c r="A3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="C4" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -1082,46 +1049,46 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="48.75">
-      <c r="A8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1130,23 +1097,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="103.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="103" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="27">
+    <row r="1" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1160,55 +1129,56 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="82.5">
-      <c r="A3" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1218,13 +1188,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="54.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="54.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1238,18 +1208,18 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="32.25">
+    <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1228,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1268,13 +1238,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="38.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="16.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="35.25">
+    <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1288,18 +1258,18 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1308,23 +1278,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="38.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="15.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="35.25">
+    <row r="1" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1338,60 +1310,60 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:4" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="6" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="6">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>